<commit_message>
change file data-test.xltx to data-test-product-purchase.xlsx
</commit_message>
<xml_diff>
--- a/data-test-product-purchase.xlsx
+++ b/data-test-product-purchase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nguyencaocuong/auto_test/DemoAuto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CA964B6-A45B-A34F-8292-662C10D88E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D0895B-E00D-D44B-A993-054412B2B323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="600" windowWidth="28040" windowHeight="16660" activeTab="7" xr2:uid="{8E52986E-B48F-1F4E-A76B-C808E969DAF3}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Overview" sheetId="5" r:id="rId5"/>
     <sheet name="Complete" sheetId="6" r:id="rId6"/>
     <sheet name="Cart" sheetId="7" r:id="rId7"/>
-    <sheet name="dd" sheetId="8" r:id="rId8"/>
+    <sheet name="Messages" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="74">
   <si>
     <t>standard_user</t>
   </si>
@@ -253,6 +253,18 @@
   </si>
   <si>
     <t>xpath=//button[@id="checkout" and @name="checkout"]</t>
+  </si>
+  <si>
+    <t>✅ The total number of products in the cart: {0}</t>
+  </si>
+  <si>
+    <t>msg_pass_cart_badge</t>
+  </si>
+  <si>
+    <t>msg_pass_cart_badge2</t>
+  </si>
+  <si>
+    <t>msg_pass_cart_badge3</t>
   </si>
 </sst>
 </file>
@@ -1165,14 +1177,42 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBDCE08D-DFEA-FD4D-A29D-DC3EF98D8CC5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="34">
+      <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="85">
+      <c r="A2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add messages to Excel file
</commit_message>
<xml_diff>
--- a/data-test-product-purchase.xlsx
+++ b/data-test-product-purchase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nguyencaocuong/auto_test/DemoAuto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D0895B-E00D-D44B-A993-054412B2B323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728A37B0-1AF8-7B40-ACB0-820A7A78A7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="600" windowWidth="28040" windowHeight="16660" activeTab="7" xr2:uid="{8E52986E-B48F-1F4E-A76B-C808E969DAF3}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="96">
   <si>
     <t>standard_user</t>
   </si>
@@ -261,17 +261,88 @@
     <t>msg_pass_cart_badge</t>
   </si>
   <si>
-    <t>msg_pass_cart_badge2</t>
-  </si>
-  <si>
-    <t>msg_pass_cart_badge3</t>
+    <t>msg_not_pass_cart_badge2</t>
+  </si>
+  <si>
+    <t>❌ The total number off products in the cart is incorrect!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	The number of products displayed is incorrect; 
+	{0} products were added, but {1} are shown.</t>
+  </si>
+  <si>
+    <t>✅ Number of products on display: {0}</t>
+  </si>
+  <si>
+    <t>\tProduct name number {0} is displayed incorrectly.\n\tAdded name: {1}.\n\tDisplayed name: {2}.</t>
+  </si>
+  <si>
+    <t>Name Product {0}: {1}</t>
+  </si>
+  <si>
+    <t>msg_not_pass_display_priceProduct</t>
+  </si>
+  <si>
+    <t>msg_pass_display_priceProduct</t>
+  </si>
+  <si>
+    <t>msg_not_pass_display_nameProduct</t>
+  </si>
+  <si>
+    <t>msg_pass_display_sizeProduct</t>
+  </si>
+  <si>
+    <t>msg_not_pass_display_sizeProduct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Product price number {0} is displayed incorrectly.
+	Added price: {1}.
+	Displayed price: {2}.</t>
+  </si>
+  <si>
+    <t>Price Product {0}: {1}</t>
+  </si>
+  <si>
+    <t>msg_not_pass_display_quantityProduct</t>
+  </si>
+  <si>
+    <t>msg_pass_display_quantityProduct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Product quantity number {0} is displayed incorrectly.
+	Added quantity: {1}.
+	Displayed quantity: {2}.</t>
+  </si>
+  <si>
+    <t>Quantity Product: {1}</t>
+  </si>
+  <si>
+    <t>msg_not_pass_display_btn</t>
+  </si>
+  <si>
+    <t>msg_pass_display_btn</t>
+  </si>
+  <si>
+    <t>❌ Button {0} is not displayed</t>
+  </si>
+  <si>
+    <t>✅ Button {0} is displayed</t>
+  </si>
+  <si>
+    <t>msg_pass_click_btn</t>
+  </si>
+  <si>
+    <t>✅ Button {0} is clicked</t>
+  </si>
+  <si>
+    <t>msg_pass_display_nameProduct</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -286,6 +357,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -311,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -323,6 +401,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1177,10 +1258,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBDCE08D-DFEA-FD4D-A29D-DC3EF98D8CC5}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1189,7 +1270,7 @@
     <col min="2" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="34">
+    <row r="1" spans="1:13" ht="68">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
@@ -1197,18 +1278,78 @@
         <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="85">
+        <v>82</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="187">
       <c r="A2" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>